<commit_message>
removed Data Table from Excel file
</commit_message>
<xml_diff>
--- a/explore_census_adj.xlsx
+++ b/explore_census_adj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isken\Documents\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33317B4-C18F-4DE7-B21D-972F50847B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9CAD92-DA82-48DC-B168-81C3F19EB16A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8985" tabRatio="780" xr2:uid="{5831E6B1-140F-4CFC-A885-73B56A2DEAC1}"/>
   </bookViews>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>day</t>
   </si>
@@ -335,13 +335,7 @@
     <t>&lt;-- This is day in which to start applying social distancing rate</t>
   </si>
   <si>
-    <t>gap</t>
-  </si>
-  <si>
-    <t>mingap_t</t>
-  </si>
-  <si>
-    <t>&lt;- This is decision variable in Solver model. Can do this with Data Table too.</t>
+    <t xml:space="preserve">&lt;- This is decision variable in Solver model. </t>
   </si>
 </sst>
 </file>
@@ -8627,64 +8621,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E37E87-2EB5-4B75-B179-5255268F651C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9667875" y="4810125"/>
-          <a:ext cx="238125" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8673353" cy="6297706"/>
@@ -8716,7 +8652,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -8749,7 +8685,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8790,7 +8726,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -8823,7 +8759,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -8856,7 +8792,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -9290,9 +9226,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A8ED5C-2B82-4BE0-8FF2-889EAE1F391A}">
-  <dimension ref="A2:J150"/>
+  <dimension ref="A2:H149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -9396,7 +9332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>13</v>
       </c>
@@ -9408,8 +9344,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>18</v>
       </c>
@@ -9417,7 +9353,7 @@
         <v>43917</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>19</v>
       </c>
@@ -9426,7 +9362,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>22</v>
       </c>
@@ -9437,7 +9373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>26</v>
       </c>
@@ -9448,7 +9384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>20</v>
       </c>
@@ -9462,7 +9398,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>25</v>
       </c>
@@ -9470,10 +9406,10 @@
         <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>34</v>
       </c>
@@ -9492,16 +9428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="6">
-        <f>INDEX(I30:I150,MATCH(J29,J30:J150,0))</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>15</v>
       </c>
@@ -9521,7 +9448,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>43831</v>
       </c>
@@ -9533,15 +9460,8 @@
         <v>0</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="I29" t="s">
-        <v>42</v>
-      </c>
-      <c r="J29">
-        <f>E26</f>
-        <v>1.8854022788334532</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>43832</v>
       </c>
@@ -9562,15 +9482,8 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <f t="dataTable" ref="J30:J150" dt2D="0" dtr="0" r1="E25"/>
-        <v>7181756.4045217615</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>43833</v>
       </c>
@@ -9591,14 +9504,8 @@
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
-        <v>5943712.6444166927</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>43834</v>
       </c>
@@ -9619,14 +9526,8 @@
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="J32">
-        <v>4919088.9620188465</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>43835</v>
       </c>
@@ -9647,14 +9548,8 @@
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33">
-        <v>3</v>
-      </c>
-      <c r="J33">
-        <v>4071094.953760657</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>43836</v>
       </c>
@@ -9675,14 +9570,8 @@
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34">
-        <v>4</v>
-      </c>
-      <c r="J34">
-        <v>3369282.3269443987</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>43837</v>
       </c>
@@ -9703,14 +9592,8 @@
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35">
-        <v>5</v>
-      </c>
-      <c r="J35">
-        <v>2788451.6154509978</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>43838</v>
       </c>
@@ -9731,14 +9614,8 @@
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36">
-        <v>6</v>
-      </c>
-      <c r="J36">
-        <v>2307747.3611767981</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>43839</v>
       </c>
@@ -9759,14 +9636,8 @@
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37">
-        <v>7</v>
-      </c>
-      <c r="J37">
-        <v>1909909.2725482185</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>43840</v>
       </c>
@@ -9787,14 +9658,8 @@
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38">
-        <v>8</v>
-      </c>
-      <c r="J38">
-        <v>1580652.4720178815</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>43841</v>
       </c>
@@ -9815,14 +9680,8 @@
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39">
-        <v>9</v>
-      </c>
-      <c r="J39">
-        <v>1308154.5795481533</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>43842</v>
       </c>
@@ -9843,14 +9702,8 @@
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40">
-        <v>10</v>
-      </c>
-      <c r="J40">
-        <v>1082631.2151686181</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>43843</v>
       </c>
@@ -9871,14 +9724,8 @@
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41">
-        <v>11</v>
-      </c>
-      <c r="J41">
-        <v>895984.67849231872</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>43844</v>
       </c>
@@ -9899,14 +9746,8 @@
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42">
-        <v>12</v>
-      </c>
-      <c r="J42">
-        <v>741513.19058639393</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>43845</v>
       </c>
@@ -9927,14 +9768,8 @@
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43">
-        <v>13</v>
-      </c>
-      <c r="J43">
-        <v>613670.25816031347</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>43846</v>
       </c>
@@ -9958,14 +9793,8 @@
         <v>0</v>
       </c>
       <c r="H44" s="3"/>
-      <c r="I44">
-        <v>14</v>
-      </c>
-      <c r="J44">
-        <v>507865.51973989193</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>43847</v>
       </c>
@@ -9989,14 +9818,8 @@
         <v>0</v>
       </c>
       <c r="H45" s="3"/>
-      <c r="I45">
-        <v>15</v>
-      </c>
-      <c r="J45">
-        <v>420299.92295818171</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>43848</v>
       </c>
@@ -10020,14 +9843,8 @@
         <v>0</v>
       </c>
       <c r="H46" s="3"/>
-      <c r="I46">
-        <v>16</v>
-      </c>
-      <c r="J46">
-        <v>347829.3147962956</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>43849</v>
       </c>
@@ -10051,14 +9868,8 @@
         <v>0</v>
       </c>
       <c r="H47" s="3"/>
-      <c r="I47">
-        <v>17</v>
-      </c>
-      <c r="J47">
-        <v>287851.54681001545</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>43850</v>
       </c>
@@ -10082,14 +9893,8 @@
         <v>0</v>
       </c>
       <c r="H48" s="3"/>
-      <c r="I48">
-        <v>18</v>
-      </c>
-      <c r="J48">
-        <v>238213.04171315974</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>43851</v>
       </c>
@@ -10113,14 +9918,8 @@
         <v>0</v>
       </c>
       <c r="H49" s="3"/>
-      <c r="I49">
-        <v>19</v>
-      </c>
-      <c r="J49">
-        <v>197131.46647324332</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>43852</v>
       </c>
@@ -10144,14 +9943,8 @@
         <v>0</v>
       </c>
       <c r="H50" s="3"/>
-      <c r="I50">
-        <v>20</v>
-      </c>
-      <c r="J50">
-        <v>163131.73539955736</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>43853</v>
       </c>
@@ -10175,14 +9968,8 @@
         <v>0</v>
       </c>
       <c r="H51" s="3"/>
-      <c r="I51">
-        <v>21</v>
-      </c>
-      <c r="J51">
-        <v>134993.04533394883</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>43854</v>
       </c>
@@ -10206,14 +9993,8 @@
         <v>0</v>
       </c>
       <c r="H52" s="3"/>
-      <c r="I52">
-        <v>22</v>
-      </c>
-      <c r="J52">
-        <v>111705.04117614028</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>43855</v>
       </c>
@@ -10237,14 +10018,8 @@
         <v>0</v>
       </c>
       <c r="H53" s="3"/>
-      <c r="I53">
-        <v>23</v>
-      </c>
-      <c r="J53">
-        <v>92431.537811570161</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>43856</v>
       </c>
@@ -10268,14 +10043,8 @@
         <v>0</v>
       </c>
       <c r="H54" s="3"/>
-      <c r="I54">
-        <v>24</v>
-      </c>
-      <c r="J54">
-        <v>76480.495831892898</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>43857</v>
       </c>
@@ -10299,14 +10068,8 @@
         <v>0</v>
       </c>
       <c r="H55" s="3"/>
-      <c r="I55">
-        <v>25</v>
-      </c>
-      <c r="J55">
-        <v>63279.172988577055</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>43858</v>
       </c>
@@ -10330,14 +10093,8 @@
         <v>0</v>
       </c>
       <c r="H56" s="3"/>
-      <c r="I56">
-        <v>26</v>
-      </c>
-      <c r="J56">
-        <v>52353.559161249083</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>43859</v>
       </c>
@@ -10361,14 +10118,8 @@
         <v>0</v>
       </c>
       <c r="H57" s="3"/>
-      <c r="I57">
-        <v>27</v>
-      </c>
-      <c r="J57">
-        <v>43311.356427426697</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>43860</v>
       </c>
@@ -10392,14 +10143,8 @@
         <v>0</v>
       </c>
       <c r="H58" s="3"/>
-      <c r="I58">
-        <v>28</v>
-      </c>
-      <c r="J58">
-        <v>35827.893111614045</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>43861</v>
       </c>
@@ -10423,14 +10168,8 @@
         <v>0</v>
       </c>
       <c r="H59" s="3"/>
-      <c r="I59">
-        <v>29</v>
-      </c>
-      <c r="J59">
-        <v>29634.466039951894</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>43862</v>
       </c>
@@ -10454,14 +10193,8 @@
         <v>0</v>
       </c>
       <c r="H60" s="3"/>
-      <c r="I60">
-        <v>30</v>
-      </c>
-      <c r="J60">
-        <v>24508.692414397225</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>43863</v>
       </c>
@@ -10485,14 +10218,8 @@
         <v>0</v>
       </c>
       <c r="H61" s="3"/>
-      <c r="I61">
-        <v>31</v>
-      </c>
-      <c r="J61">
-        <v>20266.524878325756</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>43864</v>
       </c>
@@ -10516,14 +10243,8 @@
         <v>0</v>
       </c>
       <c r="H62" s="3"/>
-      <c r="I62">
-        <v>32</v>
-      </c>
-      <c r="J62">
-        <v>16755.643064431442</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>43865</v>
       </c>
@@ -10547,14 +10268,8 @@
         <v>0</v>
       </c>
       <c r="H63" s="3"/>
-      <c r="I63">
-        <v>33</v>
-      </c>
-      <c r="J63">
-        <v>13849.98434013017</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>43866</v>
       </c>
@@ -10578,14 +10293,8 @@
         <v>0</v>
       </c>
       <c r="H64" s="3"/>
-      <c r="I64">
-        <v>34</v>
-      </c>
-      <c r="J64">
-        <v>11445.217369993081</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>43867</v>
       </c>
@@ -10609,14 +10318,8 @@
         <v>0</v>
       </c>
       <c r="H65" s="3"/>
-      <c r="I65">
-        <v>35</v>
-      </c>
-      <c r="J65">
-        <v>9454.9959677693769</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>43868</v>
       </c>
@@ -10640,14 +10343,8 @@
         <v>0</v>
       </c>
       <c r="H66" s="3"/>
-      <c r="I66">
-        <v>36</v>
-      </c>
-      <c r="J66">
-        <v>7807.8587278382201</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>43869</v>
       </c>
@@ -10671,14 +10368,8 @@
         <v>0</v>
       </c>
       <c r="H67" s="3"/>
-      <c r="I67">
-        <v>37</v>
-      </c>
-      <c r="J67">
-        <v>6444.6631134524359</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>43870</v>
       </c>
@@ -10702,14 +10393,8 @@
         <v>0</v>
       </c>
       <c r="H68" s="3"/>
-      <c r="I68">
-        <v>38</v>
-      </c>
-      <c r="J68">
-        <v>5316.4618694818455</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>43871</v>
       </c>
@@ -10733,14 +10418,8 @@
         <v>0</v>
       </c>
       <c r="H69" s="3"/>
-      <c r="I69">
-        <v>39</v>
-      </c>
-      <c r="J69">
-        <v>4382.7455095812265</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
         <v>43872</v>
       </c>
@@ -10764,14 +10443,8 @@
         <v>0</v>
       </c>
       <c r="H70" s="3"/>
-      <c r="I70">
-        <v>40</v>
-      </c>
-      <c r="J70">
-        <v>3609.9877720717705</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>43873</v>
       </c>
@@ -10795,14 +10468,8 @@
         <v>0</v>
       </c>
       <c r="H71" s="3"/>
-      <c r="I71">
-        <v>41</v>
-      </c>
-      <c r="J71">
-        <v>2970.4418172977835</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
         <v>43874</v>
       </c>
@@ -10826,14 +10493,8 @@
         <v>0</v>
       </c>
       <c r="H72" s="3"/>
-      <c r="I72">
-        <v>42</v>
-      </c>
-      <c r="J72">
-        <v>2441.1439424088039</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="1">
         <v>43875</v>
       </c>
@@ -10857,14 +10518,8 @@
         <v>0</v>
       </c>
       <c r="H73" s="3"/>
-      <c r="I73">
-        <v>43</v>
-      </c>
-      <c r="J73">
-        <v>2003.0890406918561</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="1">
         <v>43876</v>
       </c>
@@ -10888,14 +10543,8 @@
         <v>0</v>
       </c>
       <c r="H74" s="3"/>
-      <c r="I74">
-        <v>44</v>
-      </c>
-      <c r="J74">
-        <v>1640.5481992828613</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="1">
         <v>43877</v>
       </c>
@@ -10919,14 +10568,8 @@
         <v>0</v>
       </c>
       <c r="H75" s="3"/>
-      <c r="I75">
-        <v>45</v>
-      </c>
-      <c r="J75">
-        <v>1340.503932743708</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
         <v>43878</v>
       </c>
@@ -10950,14 +10593,8 @@
         <v>0</v>
       </c>
       <c r="H76" s="3"/>
-      <c r="I76">
-        <v>46</v>
-      </c>
-      <c r="J76">
-        <v>1092.1827738554141</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1">
         <v>43879</v>
       </c>
@@ -10981,14 +10618,8 @@
         <v>0</v>
       </c>
       <c r="H77" s="3"/>
-      <c r="I77">
-        <v>47</v>
-      </c>
-      <c r="J77">
-        <v>886.66843871120886</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="1">
         <v>43880</v>
       </c>
@@ -11012,14 +10643,8 @@
         <v>0</v>
       </c>
       <c r="H78" s="3"/>
-      <c r="I78">
-        <v>48</v>
-      </c>
-      <c r="J78">
-        <v>716.58167631507877</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="1">
         <v>43881</v>
       </c>
@@ -11043,14 +10668,8 @@
         <v>0</v>
       </c>
       <c r="H79" s="3"/>
-      <c r="I79">
-        <v>49</v>
-      </c>
-      <c r="J79">
-        <v>575.81530728248379</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
         <v>43882</v>
       </c>
@@ -11074,14 +10693,8 @@
         <v>0</v>
       </c>
       <c r="H80" s="3"/>
-      <c r="I80">
-        <v>50</v>
-      </c>
-      <c r="J80">
-        <v>459.31493787412592</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
         <v>43883</v>
       </c>
@@ -11105,14 +10718,8 @@
         <v>0</v>
       </c>
       <c r="H81" s="3"/>
-      <c r="I81">
-        <v>51</v>
-      </c>
-      <c r="J81">
-        <v>362.89747562402596</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>43884</v>
       </c>
@@ -11136,14 +10743,8 @@
         <v>0</v>
       </c>
       <c r="H82" s="3"/>
-      <c r="I82">
-        <v>52</v>
-      </c>
-      <c r="J82">
-        <v>283.10093013699975</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
         <v>43885</v>
       </c>
@@ -11167,14 +10768,8 @@
         <v>0</v>
       </c>
       <c r="H83" s="3"/>
-      <c r="I83">
-        <v>53</v>
-      </c>
-      <c r="J83">
-        <v>217.06010596402717</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
         <v>43886</v>
       </c>
@@ -11198,14 +10793,8 @@
         <v>0</v>
       </c>
       <c r="H84" s="3"/>
-      <c r="I84">
-        <v>54</v>
-      </c>
-      <c r="J84">
-        <v>162.40372415167673</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>43887</v>
       </c>
@@ -11229,14 +10818,8 @@
         <v>0</v>
       </c>
       <c r="H85" s="3"/>
-      <c r="I85">
-        <v>55</v>
-      </c>
-      <c r="J85">
-        <v>117.16927848526453</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>43888</v>
       </c>
@@ -11260,14 +10843,8 @@
         <v>0</v>
       </c>
       <c r="H86" s="3"/>
-      <c r="I86">
-        <v>56</v>
-      </c>
-      <c r="J86">
-        <v>79.732569231941</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
         <v>43889</v>
       </c>
@@ -11291,14 +10868,8 @@
         <v>0</v>
       </c>
       <c r="H87" s="3"/>
-      <c r="I87">
-        <v>57</v>
-      </c>
-      <c r="J87">
-        <v>48.749384204020174</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
         <v>43890</v>
       </c>
@@ -11322,14 +10893,8 @@
         <v>0</v>
       </c>
       <c r="H88" s="3"/>
-      <c r="I88">
-        <v>58</v>
-      </c>
-      <c r="J88">
-        <v>23.107233127689796</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
         <v>43891</v>
       </c>
@@ -11353,14 +10918,8 @@
         <v>1</v>
       </c>
       <c r="H89" s="3"/>
-      <c r="I89">
-        <v>59</v>
-      </c>
-      <c r="J89">
-        <v>1.8854022788334532</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
         <v>43892</v>
       </c>
@@ -11384,14 +10943,8 @@
         <v>2.2082911818002908</v>
       </c>
       <c r="H90" s="3"/>
-      <c r="I90">
-        <v>60</v>
-      </c>
-      <c r="J90">
-        <v>15.678104902636505</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
         <v>43893</v>
       </c>
@@ -11415,14 +10968,8 @@
         <v>3.6682587618166345</v>
       </c>
       <c r="H91" s="3"/>
-      <c r="I91">
-        <v>61</v>
-      </c>
-      <c r="J91">
-        <v>30.213928258809034</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <v>43894</v>
       </c>
@@ -11446,14 +10993,8 @@
         <v>5.4323247144646931</v>
       </c>
       <c r="H92" s="3"/>
-      <c r="I92">
-        <v>62</v>
-      </c>
-      <c r="J92">
-        <v>42.243994831433476</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
         <v>43895</v>
       </c>
@@ -11477,14 +11018,8 @@
         <v>7.5638300491634709</v>
       </c>
       <c r="H93" s="3"/>
-      <c r="I93">
-        <v>63</v>
-      </c>
-      <c r="J93">
-        <v>52.200259309587047</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>43896</v>
       </c>
@@ -11508,14 +11043,8 @@
         <v>10.139309149040281</v>
       </c>
       <c r="H94" s="3"/>
-      <c r="I94">
-        <v>64</v>
-      </c>
-      <c r="J94">
-        <v>60.440213906722519</v>
-      </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>43897</v>
       </c>
@@ -11539,14 +11068,8 @@
         <v>13.251237834332382</v>
       </c>
       <c r="H95" s="3"/>
-      <c r="I95">
-        <v>65</v>
-      </c>
-      <c r="J95">
-        <v>67.259724568762081</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
         <v>43898</v>
       </c>
@@ -11570,14 +11093,8 @@
         <v>17.011353823162199</v>
       </c>
       <c r="H96" s="3"/>
-      <c r="I96">
-        <v>66</v>
-      </c>
-      <c r="J96">
-        <v>72.90365441345304</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1">
         <v>43899</v>
       </c>
@@ -11601,14 +11118,8 @@
         <v>21.554668815011549</v>
       </c>
       <c r="H97" s="3"/>
-      <c r="I97">
-        <v>67</v>
-      </c>
-      <c r="J97">
-        <v>77.574655848952887</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="1">
         <v>43900</v>
       </c>
@@ -11632,14 +11143,8 @@
         <v>27.04431625580418</v>
       </c>
       <c r="H98" s="3"/>
-      <c r="I98">
-        <v>68</v>
-      </c>
-      <c r="J98">
-        <v>81.440447063732989</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
         <v>43901</v>
       </c>
@@ -11663,14 +11168,8 @@
         <v>33.677408849706445</v>
       </c>
       <c r="H99" s="3"/>
-      <c r="I99">
-        <v>69</v>
-      </c>
-      <c r="J99">
-        <v>84.639834159333816</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="1">
         <v>43902</v>
       </c>
@@ -11694,14 +11193,8 @@
         <v>41.692116138983373</v>
       </c>
       <c r="H100" s="3"/>
-      <c r="I100">
-        <v>70</v>
-      </c>
-      <c r="J100">
-        <v>87.287695158231358</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="1">
         <v>43903</v>
       </c>
@@ -11725,14 +11218,8 @@
         <v>51.376216281327196</v>
       </c>
       <c r="H101" s="3"/>
-      <c r="I101">
-        <v>71</v>
-      </c>
-      <c r="J101">
-        <v>89.479104843893694</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="1">
         <v>43904</v>
       </c>
@@ -11756,14 +11243,8 @@
         <v>63.077429086992176</v>
       </c>
       <c r="H102" s="3"/>
-      <c r="I102">
-        <v>72</v>
-      </c>
-      <c r="J102">
-        <v>91.292748540603668</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
         <v>43905</v>
       </c>
@@ -11787,14 +11268,8 @@
         <v>76.21590133644581</v>
       </c>
       <c r="H103" s="3"/>
-      <c r="I103">
-        <v>73</v>
-      </c>
-      <c r="J103">
-        <v>92.79374740911129</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="1">
         <v>43906</v>
       </c>
@@ -11818,14 +11293,8 @@
         <v>92.091001497788483</v>
       </c>
       <c r="H104" s="3"/>
-      <c r="I104">
-        <v>74</v>
-      </c>
-      <c r="J104">
-        <v>94.035996703913895</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="1">
         <v>43907</v>
       </c>
@@ -11849,14 +11318,8 @@
         <v>111.27274503293518</v>
       </c>
       <c r="H105" s="3"/>
-      <c r="I105">
-        <v>75</v>
-      </c>
-      <c r="J105">
-        <v>95.064100950236138</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="1">
         <v>43908</v>
       </c>
@@ -11880,14 +11343,8 @@
         <v>134.44987659800768</v>
       </c>
       <c r="H106" s="3"/>
-      <c r="I106">
-        <v>76</v>
-      </c>
-      <c r="J106">
-        <v>95.914975525676155</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="1">
         <v>43909</v>
       </c>
@@ -11911,14 +11368,8 @@
         <v>162.45460028750998</v>
       </c>
       <c r="H107" s="3"/>
-      <c r="I107">
-        <v>77</v>
-      </c>
-      <c r="J107">
-        <v>96.619172153323703</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="1">
         <v>43910</v>
       </c>
@@ -11942,14 +11393,8 @@
         <v>196.29246097028931</v>
       </c>
       <c r="H108" s="3"/>
-      <c r="I108">
-        <v>78</v>
-      </c>
-      <c r="J108">
-        <v>97.2019758998497</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="1">
         <v>43911</v>
       </c>
@@ -11973,14 +11418,8 @@
         <v>237.17844964427832</v>
       </c>
       <c r="H109" s="3"/>
-      <c r="I109">
-        <v>79</v>
-      </c>
-      <c r="J109">
-        <v>97.684313067665201</v>
-      </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="1">
         <v>43912</v>
       </c>
@@ -12004,14 +11443,8 @@
         <v>286.5806292182458</v>
       </c>
       <c r="H110" s="3"/>
-      <c r="I110">
-        <v>80</v>
-      </c>
-      <c r="J110">
-        <v>98.08350258016074</v>
-      </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="1">
         <v>43913</v>
       </c>
@@ -12035,14 +11468,8 @@
         <v>341.2873247906831</v>
       </c>
       <c r="H111" s="3"/>
-      <c r="I111">
-        <v>81</v>
-      </c>
-      <c r="J111">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="1">
         <v>43914</v>
       </c>
@@ -12066,14 +11493,8 @@
         <v>401.83251867312248</v>
       </c>
       <c r="H112" s="3"/>
-      <c r="I112">
-        <v>82</v>
-      </c>
-      <c r="J112">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="1">
         <v>43915</v>
       </c>
@@ -12097,14 +11518,8 @@
         <v>468.79604196257344</v>
       </c>
       <c r="H113" s="3"/>
-      <c r="I113">
-        <v>83</v>
-      </c>
-      <c r="J113">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="1">
         <v>43916</v>
       </c>
@@ -12128,14 +11543,8 @@
         <v>542.80563822191823</v>
       </c>
       <c r="H114" s="3"/>
-      <c r="I114">
-        <v>84</v>
-      </c>
-      <c r="J114">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" s="1">
         <v>43917</v>
       </c>
@@ -12155,18 +11564,12 @@
         <v>1.8854022788334532</v>
       </c>
       <c r="G115" s="3">
-        <f t="shared" si="10"/>
+        <f>SUM(E101:E114)</f>
         <v>624.5385997458327</v>
       </c>
       <c r="H115" s="3"/>
-      <c r="I115">
-        <v>85</v>
-      </c>
-      <c r="J115">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" s="1">
         <v>43918</v>
       </c>
@@ -12190,14 +11593,8 @@
         <v>714.72278921900113</v>
       </c>
       <c r="H116" s="3"/>
-      <c r="I116">
-        <v>86</v>
-      </c>
-      <c r="J116">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" s="1">
         <v>43919</v>
       </c>
@@ -12221,14 +11618,8 @@
         <v>814.13680934145202</v>
       </c>
       <c r="H117" s="3"/>
-      <c r="I117">
-        <v>87</v>
-      </c>
-      <c r="J117">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1">
         <v>43920</v>
       </c>
@@ -12252,14 +11643,8 @@
         <v>923.60902101377849</v>
       </c>
       <c r="H118" s="3"/>
-      <c r="I118">
-        <v>88</v>
-      </c>
-      <c r="J118">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="1">
         <v>43921</v>
       </c>
@@ -12283,14 +11668,8 @@
         <v>1044.0150343479634</v>
       </c>
       <c r="H119" s="3"/>
-      <c r="I119">
-        <v>89</v>
-      </c>
-      <c r="J119">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="1">
         <v>43922</v>
       </c>
@@ -12314,14 +11693,8 @@
         <v>1176.2732029452891</v>
       </c>
       <c r="H120" s="3"/>
-      <c r="I120">
-        <v>90</v>
-      </c>
-      <c r="J120">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1">
         <v>43923</v>
       </c>
@@ -12345,14 +11718,8 @@
         <v>1321.337536733759</v>
       </c>
       <c r="H121" s="3"/>
-      <c r="I121">
-        <v>91</v>
-      </c>
-      <c r="J121">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="1">
         <v>43924</v>
       </c>
@@ -12376,14 +11743,8 @@
         <v>1480.1873075377728</v>
       </c>
       <c r="H122" s="3"/>
-      <c r="I122">
-        <v>92</v>
-      </c>
-      <c r="J122">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
         <v>43925</v>
       </c>
@@ -12407,14 +11768,8 @@
         <v>1653.8124488255644</v>
       </c>
       <c r="H123" s="3"/>
-      <c r="I123">
-        <v>93</v>
-      </c>
-      <c r="J123">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="1">
         <v>43926</v>
       </c>
@@ -12438,14 +11793,8 @@
         <v>1843.1936399081167</v>
       </c>
       <c r="H124" s="3"/>
-      <c r="I124">
-        <v>94</v>
-      </c>
-      <c r="J124">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="1">
         <v>43927</v>
       </c>
@@ -12453,7 +11802,7 @@
         <v>96</v>
       </c>
       <c r="D125" s="2">
-        <f t="shared" ref="D125:D156" si="11">IF(C125&lt;tzero_trial,0,EXP(lambda1*(C125-tzero_trial)))</f>
+        <f t="shared" ref="D125:D149" si="11">IF(C125&lt;tzero_trial,0,EXP(lambda1*(C125-tzero_trial)))</f>
         <v>1097.3607472261767</v>
       </c>
       <c r="E125" s="2">
@@ -12469,14 +11818,8 @@
         <v>2054.261229325205</v>
       </c>
       <c r="H125" s="3"/>
-      <c r="I125">
-        <v>95</v>
-      </c>
-      <c r="J125">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="1">
         <v>43928</v>
       </c>
@@ -12488,11 +11831,11 @@
         <v>1325.931314127168</v>
       </c>
       <c r="E126" s="2">
-        <f t="shared" ref="E126:E157" si="12">IF(C126&lt;=tprime,D126,INDEX($D$30:$D$149,tprime)*EXP(lambda2*(C126-tprime)))</f>
+        <f t="shared" ref="E126:E149" si="12">IF(C126&lt;=tprime,D126,INDEX($D$30:$D$149,tprime)*EXP(lambda2*(C126-tprime)))</f>
         <v>335.77142658487099</v>
       </c>
       <c r="F126">
-        <f t="shared" ref="F126:F157" si="13">ABS(E126-admrate_today)</f>
+        <f t="shared" ref="F126:F149" si="13">ABS(E126-admrate_today)</f>
         <v>235.77142658487099</v>
       </c>
       <c r="G126" s="3">
@@ -12500,14 +11843,8 @@
         <v>2289.4985675618273</v>
       </c>
       <c r="H126" s="3"/>
-      <c r="I126">
-        <v>96</v>
-      </c>
-      <c r="J126">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="1">
         <v>43929</v>
       </c>
@@ -12531,14 +11868,8 @@
         <v>2551.6733782633446</v>
       </c>
       <c r="H127" s="3"/>
-      <c r="I127">
-        <v>97</v>
-      </c>
-      <c r="J127">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" s="1">
         <v>43930</v>
       </c>
@@ -12562,14 +11893,8 @@
         <v>2843.8703223438652</v>
       </c>
       <c r="H128" s="3"/>
-      <c r="I128">
-        <v>98</v>
-      </c>
-      <c r="J128">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="1">
         <v>43931</v>
       </c>
@@ -12593,14 +11918,8 @@
         <v>3169.5272910722515</v>
       </c>
       <c r="H129" s="3"/>
-      <c r="I129">
-        <v>99</v>
-      </c>
-      <c r="J129">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="1">
         <v>43932</v>
       </c>
@@ -12624,14 +11943,8 @@
         <v>3532.4758551480495</v>
       </c>
       <c r="H130" s="3"/>
-      <c r="I130">
-        <v>100</v>
-      </c>
-      <c r="J130">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="1">
         <v>43933</v>
       </c>
@@ -12655,14 +11968,8 @@
         <v>3936.9863456775934</v>
       </c>
       <c r="H131" s="3"/>
-      <c r="I131">
-        <v>101</v>
-      </c>
-      <c r="J131">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="1">
         <v>43934</v>
       </c>
@@ -12686,14 +11993,8 @@
         <v>4387.8180974579354</v>
       </c>
       <c r="H132" s="3"/>
-      <c r="I132">
-        <v>102</v>
-      </c>
-      <c r="J132">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="1">
         <v>43935</v>
       </c>
@@ -12717,14 +12018,8 @@
         <v>4890.2754457142419</v>
       </c>
       <c r="H133" s="3"/>
-      <c r="I133">
-        <v>103</v>
-      </c>
-      <c r="J133">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="134" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="1">
         <v>43936</v>
       </c>
@@ -12748,14 +12043,8 @@
         <v>5450.2701351294781</v>
       </c>
       <c r="H134" s="3"/>
-      <c r="I134">
-        <v>104</v>
-      </c>
-      <c r="J134">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="135" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="1">
         <v>43937</v>
       </c>
@@ -12779,14 +12068,8 @@
         <v>6074.3908754501063</v>
       </c>
       <c r="H135" s="3"/>
-      <c r="I135">
-        <v>105</v>
-      </c>
-      <c r="J135">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="136" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" s="1">
         <v>43938</v>
       </c>
@@ -12810,14 +12093,8 @@
         <v>6769.9808620357398</v>
       </c>
       <c r="H136" s="3"/>
-      <c r="I136">
-        <v>106</v>
-      </c>
-      <c r="J136">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="137" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" s="1">
         <v>43939</v>
       </c>
@@ -12841,14 +12118,8 @@
         <v>7545.2241734335257</v>
       </c>
       <c r="H137" s="3"/>
-      <c r="I137">
-        <v>107</v>
-      </c>
-      <c r="J137">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="1">
         <v>43940</v>
       </c>
@@ -12872,14 +12143,8 @@
         <v>8409.2420625021678</v>
       </c>
       <c r="H138" s="3"/>
-      <c r="I138">
-        <v>108</v>
-      </c>
-      <c r="J138">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="1">
         <v>43941</v>
       </c>
@@ -12903,14 +12168,8 @@
         <v>9372.20027401466</v>
       </c>
       <c r="H139" s="3"/>
-      <c r="I139">
-        <v>109</v>
-      </c>
-      <c r="J139">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="140" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" s="1">
         <v>43942</v>
       </c>
@@ -12934,14 +12193,8 @@
         <v>10445.428651402648</v>
       </c>
       <c r="H140" s="3"/>
-      <c r="I140">
-        <v>110</v>
-      </c>
-      <c r="J140">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="141" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="1">
         <v>43943</v>
       </c>
@@ -12965,14 +12218,8 @@
         <v>11641.554439895306</v>
       </c>
       <c r="H141" s="3"/>
-      <c r="I141">
-        <v>111</v>
-      </c>
-      <c r="J141">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="142" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="1">
         <v>43944</v>
       </c>
@@ -12996,14 +12243,8 @@
         <v>12974.650854452702</v>
       </c>
       <c r="H142" s="3"/>
-      <c r="I142">
-        <v>112</v>
-      </c>
-      <c r="J142">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="143" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" s="1">
         <v>43945</v>
       </c>
@@ -13027,14 +12268,8 @@
         <v>14460.402660494205</v>
       </c>
       <c r="H143" s="3"/>
-      <c r="I143">
-        <v>113</v>
-      </c>
-      <c r="J143">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="144" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" s="1">
         <v>43946</v>
       </c>
@@ -13058,14 +12293,8 @@
         <v>16116.290715589226</v>
       </c>
       <c r="H144" s="3"/>
-      <c r="I144">
-        <v>114</v>
-      </c>
-      <c r="J144">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" s="1">
         <v>43947</v>
       </c>
@@ -13089,14 +12318,8 @@
         <v>17961.79764336595</v>
       </c>
       <c r="H145" s="3"/>
-      <c r="I145">
-        <v>115</v>
-      </c>
-      <c r="J145">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" s="1">
         <v>43948</v>
       </c>
@@ -13120,14 +12343,8 @@
         <v>20018.637059528315</v>
       </c>
       <c r="H146" s="3"/>
-      <c r="I146">
-        <v>116</v>
-      </c>
-      <c r="J146">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" s="1">
         <v>43949</v>
       </c>
@@ -13151,14 +12368,8 @@
         <v>22311.009046977699</v>
       </c>
       <c r="H147" s="3"/>
-      <c r="I147">
-        <v>117</v>
-      </c>
-      <c r="J147">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" s="1">
         <v>43950</v>
       </c>
@@ -13182,14 +12393,8 @@
         <v>24865.884885873922</v>
       </c>
       <c r="H148" s="3"/>
-      <c r="I148">
-        <v>118</v>
-      </c>
-      <c r="J148">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" s="1">
         <v>43951</v>
       </c>
@@ -13213,25 +12418,10 @@
         <v>27713.324388673995</v>
       </c>
       <c r="H149" s="3"/>
-      <c r="I149">
-        <v>119</v>
-      </c>
-      <c r="J149">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="150" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I150">
-        <v>120</v>
-      </c>
-      <c r="J150">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>